<commit_message>
IOSAPP14-25 Removed unneeded Template.rtf file and rescrubbed Office document metadata using Office 2010 on Windows
</commit_message>
<xml_diff>
--- a/Resources-Branding/Shared/Templates/Template.xlsx
+++ b/Resources-Branding/Shared/Templates/Template.xlsx
@@ -1,28 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr filterPrivacy="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="880" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -56,12 +53,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -205,16 +202,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -336,63 +337,43 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>